<commit_message>
changed date in excel sheet file
</commit_message>
<xml_diff>
--- a/visitors.xlsx
+++ b/visitors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Record Id</t>
   </si>
@@ -37,13 +37,7 @@
     <t>email</t>
   </si>
   <si>
-    <t>updated</t>
-  </si>
-  <si>
-    <t>created At</t>
-  </si>
-  <si>
-    <t>updated At</t>
+    <t>created At3</t>
   </si>
   <si>
     <t>"62e26c60d9ae149bcb01795f"</t>
@@ -79,6 +73,9 @@
     <t>123123</t>
   </si>
   <si>
+    <t>Sat Jul 30 2022 18:31:07 GMT+0300 (Eastern European Summer Time)3</t>
+  </si>
+  <si>
     <t>"62e54f03dc06ad8e59b42bb2"</t>
   </si>
   <si>
@@ -89,6 +86,33 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>Sat Jul 30 2022 18:32:19 GMT+0300 (Eastern European Summer Time)3</t>
+  </si>
+  <si>
+    <t>"62e66c45b301c57149bdf071"</t>
+  </si>
+  <si>
+    <t>123123123</t>
+  </si>
+  <si>
+    <t>now@hotmail.com</t>
+  </si>
+  <si>
+    <t>Sun Jul 31 2022 14:49:25 GMT+0300 (Eastern European Summer Time)3</t>
+  </si>
+  <si>
+    <t>"62e6709542df06499605257d"</t>
+  </si>
+  <si>
+    <t>mouaz last test time</t>
+  </si>
+  <si>
+    <t>instagram</t>
+  </si>
+  <si>
+    <t>Sun Jul 31 2022 15:07:49 GMT+0300 (Eastern European Summer Time)3</t>
   </si>
 </sst>
 </file>
@@ -127,10 +151,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,14 +493,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="9" width="30" customWidth="1"/>
-    <col min="10" max="11" width="30" style="1" customWidth="1"/>
+    <col min="1" max="8" width="30" customWidth="1"/>
+    <col min="9" max="9" width="30" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,121 +525,145 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2">
-        <v>44770.458894814816</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="2">
-        <v>44770.519315115744</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2">
-        <v>44772.64661299768</v>
-      </c>
-      <c r="J4" s="1">
-        <v>44772.646613206016</v>
-      </c>
-      <c r="K4" s="1">
-        <v>44772.646613206016</v>
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="2">
-        <v>44772.64744453704</v>
-      </c>
-      <c r="J5" s="1">
-        <v>44772.6474446412</v>
-      </c>
-      <c r="K5" s="1">
-        <v>44772.6474446412</v>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>